<commit_message>
commit bỏ qua các file không cần
</commit_message>
<xml_diff>
--- a/Nguyen_Truong_Giang/Project-WPF/Ex WPF/Ex WPF/Excel/Data.xlsx
+++ b/Nguyen_Truong_Giang/Project-WPF/Ex WPF/Ex WPF/Excel/Data.xlsx
@@ -5,18 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Nguyen_Truong_Giang\Project-WPF\Ex WPF\Ex WPF\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Training\Nguyen_Truong_Giang\Project-WPF\Ex WPF\Ex WPF\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3B1896-DF33-42FE-89E6-1615EB3BE30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4A5641-314C-402F-87F6-63A73AE9A1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8928" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="1" r:id="rId1"/>
     <sheet name="Teacher" sheetId="2" r:id="rId2"/>
     <sheet name="Employees" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Shee6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -118,6 +120,12 @@
   </si>
   <si>
     <t>TaxFactor</t>
+  </si>
+  <si>
+    <t>TaxFactor1</t>
+  </si>
+  <si>
+    <t>TaxFactor2</t>
   </si>
 </sst>
 </file>
@@ -641,7 +649,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E6" sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,7 +771,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E6" sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -886,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31F1C6F-34DE-4819-8E10-5DE0EF3B6385}">
   <dimension ref="B1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1006,4 +1014,282 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071E9579-BF51-4674-8E28-EA9693BEDAA0}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>201</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>202</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3">
+        <v>29</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>203</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>204</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="3">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>205</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D4179A-2335-4159-A336-A0025397B68B}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="21.5546875" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>101</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3">
+        <v>32</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>102</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3">
+        <v>37</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>103</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>104</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>105</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>